<commit_message>
Factor demand-distance fixed. Numbers of iterations as variable. The tracking of test[0] must be checked
</commit_message>
<xml_diff>
--- a/Results_Summary.xlsx
+++ b/Results_Summary.xlsx
@@ -160,6 +160,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -181,6 +182,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -276,13 +278,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P28" activeCellId="0" sqref="P28"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.65"/>
@@ -391,6 +393,10 @@
         <v>1.76578</v>
       </c>
       <c r="O3" s="3"/>
+      <c r="P3" s="0" t="n">
+        <f aca="false">50000/(D3*2)</f>
+        <v>1666.66666666667</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="n">
@@ -436,6 +442,10 @@
         <v>1.63559</v>
       </c>
       <c r="O4" s="3"/>
+      <c r="P4" s="0" t="n">
+        <f aca="false">50000/(D4*2)</f>
+        <v>1666.66666666667</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="n">
@@ -481,6 +491,10 @@
         <v>4.43235</v>
       </c>
       <c r="O5" s="3"/>
+      <c r="P5" s="0" t="n">
+        <f aca="false">50000/(D5*2)</f>
+        <v>1250</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="n">
@@ -526,6 +540,10 @@
         <v>3.99178</v>
       </c>
       <c r="O6" s="3"/>
+      <c r="P6" s="0" t="n">
+        <f aca="false">50000/(D6*2)</f>
+        <v>1250</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="n">
@@ -571,6 +589,10 @@
         <v>5.50857</v>
       </c>
       <c r="O7" s="3"/>
+      <c r="P7" s="0" t="n">
+        <f aca="false">50000/(D7*2)</f>
+        <v>1190.47619047619</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
@@ -616,6 +638,10 @@
         <v>4.97322</v>
       </c>
       <c r="O8" s="3"/>
+      <c r="P8" s="0" t="n">
+        <f aca="false">50000/(D8*2)</f>
+        <v>1190.47619047619</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="n">
@@ -663,6 +689,10 @@
       <c r="O9" s="3" t="n">
         <v>20</v>
       </c>
+      <c r="P9" s="0" t="n">
+        <f aca="false">50000/(D9*2)</f>
+        <v>1136.36363636364</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="n">
@@ -710,6 +740,10 @@
       <c r="O10" s="3" t="n">
         <v>12</v>
       </c>
+      <c r="P10" s="0" t="n">
+        <f aca="false">50000/(D10*2)</f>
+        <v>1136.36363636364</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="n">
@@ -757,6 +791,10 @@
       <c r="O11" s="3" t="n">
         <v>22</v>
       </c>
+      <c r="P11" s="0" t="n">
+        <f aca="false">50000/(D11*2)</f>
+        <v>1000</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="n">
@@ -804,6 +842,10 @@
       <c r="O12" s="3" t="n">
         <v>20</v>
       </c>
+      <c r="P12" s="0" t="n">
+        <f aca="false">50000/(D12*2)</f>
+        <v>862.068965517241</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="n">
@@ -851,6 +893,10 @@
       <c r="O13" s="3" t="n">
         <v>22</v>
       </c>
+      <c r="P13" s="0" t="n">
+        <f aca="false">50000/(D13*2)</f>
+        <v>833.333333333333</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="n">
@@ -898,6 +944,10 @@
       <c r="O14" s="3" t="n">
         <v>31</v>
       </c>
+      <c r="P14" s="0" t="n">
+        <f aca="false">50000/(D14*2)</f>
+        <v>781.25</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="n">
@@ -945,6 +995,10 @@
       <c r="O15" s="3" t="n">
         <v>18</v>
       </c>
+      <c r="P15" s="0" t="n">
+        <f aca="false">50000/(D15*2)</f>
+        <v>781.25</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="n">
@@ -992,6 +1046,10 @@
       <c r="O16" s="3" t="n">
         <v>13</v>
       </c>
+      <c r="P16" s="0" t="n">
+        <f aca="false">50000/(D16*2)</f>
+        <v>781.25</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="n">
@@ -1039,6 +1097,10 @@
       <c r="O17" s="3" t="n">
         <v>20</v>
       </c>
+      <c r="P17" s="0" t="n">
+        <f aca="false">50000/(D17*2)</f>
+        <v>714.285714285714</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="n">
@@ -1086,6 +1148,10 @@
       <c r="O18" s="3" t="n">
         <v>24</v>
       </c>
+      <c r="P18" s="0" t="n">
+        <f aca="false">50000/(D18*2)</f>
+        <v>625</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="n">
@@ -1133,6 +1199,10 @@
       <c r="O19" s="3" t="n">
         <v>12</v>
       </c>
+      <c r="P19" s="0" t="n">
+        <f aca="false">50000/(D19*2)</f>
+        <v>568.181818181818</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="n">
@@ -1180,6 +1250,10 @@
       <c r="O20" s="3" t="n">
         <v>37</v>
       </c>
+      <c r="P20" s="0" t="n">
+        <f aca="false">50000/(D20*2)</f>
+        <v>500</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="n">
@@ -1227,6 +1301,10 @@
       <c r="O21" s="3" t="n">
         <v>19</v>
       </c>
+      <c r="P21" s="0" t="n">
+        <f aca="false">50000/(D21*2)</f>
+        <v>352.112676056338</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="n">
@@ -1274,6 +1352,10 @@
       <c r="O22" s="3" t="n">
         <v>41</v>
       </c>
+      <c r="P22" s="0" t="n">
+        <f aca="false">50000/(D22*2)</f>
+        <v>333.333333333333</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="n">
@@ -1321,6 +1403,10 @@
       <c r="O23" s="3" t="n">
         <v>36</v>
       </c>
+      <c r="P23" s="0" t="n">
+        <f aca="false">50000/(D23*2)</f>
+        <v>333.333333333333</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="n">
@@ -1368,6 +1454,10 @@
       <c r="O24" s="3" t="n">
         <v>33</v>
       </c>
+      <c r="P24" s="0" t="n">
+        <f aca="false">50000/(D24*2)</f>
+        <v>333.333333333333</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="n">
@@ -1415,6 +1505,10 @@
       <c r="O25" s="3" t="n">
         <v>44</v>
       </c>
+      <c r="P25" s="0" t="n">
+        <f aca="false">50000/(D25*2)</f>
+        <v>333.333333333333</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="n">
@@ -1462,6 +1556,10 @@
       <c r="O26" s="3" t="n">
         <v>45</v>
       </c>
+      <c r="P26" s="0" t="n">
+        <f aca="false">50000/(D26*2)</f>
+        <v>250</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="n">
@@ -1509,6 +1607,10 @@
       <c r="O27" s="3" t="n">
         <v>33</v>
       </c>
+      <c r="P27" s="0" t="n">
+        <f aca="false">50000/(D27*2)</f>
+        <v>250</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="n">
@@ -1555,6 +1657,10 @@
       </c>
       <c r="O28" s="3" t="n">
         <v>42</v>
+      </c>
+      <c r="P28" s="0" t="n">
+        <f aca="false">50000/(D28*2)</f>
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mathematical model tested with the first 6 instances
</commit_message>
<xml_diff>
--- a/Results_Summary.xlsx
+++ b/Results_Summary.xlsx
@@ -300,7 +300,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -427,11 +427,11 @@
   </sheetPr>
   <dimension ref="A1:AA29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y14" activeCellId="0" sqref="Y14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y6" activeCellId="0" sqref="Y6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.28"/>
@@ -800,12 +800,16 @@
         <f aca="false">M5*10</f>
         <v>25000</v>
       </c>
-      <c r="Y5" s="9"/>
+      <c r="Y5" s="9" t="n">
+        <v>285.962</v>
+      </c>
       <c r="Z5" s="11" t="n">
         <f aca="false">(Y5-J5)/J5</f>
-        <v>-1</v>
-      </c>
-      <c r="AA5" s="9"/>
+        <v>-0.0794780011073484</v>
+      </c>
+      <c r="AA5" s="9" t="n">
+        <v>211.476</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="n">
@@ -2845,7 +2849,7 @@
       </c>
       <c r="Z29" s="14" t="n">
         <f aca="false">AVERAGE(Z3:Z14)</f>
-        <v>-0.0561100497969104</v>
+        <v>0.0206001167774772</v>
       </c>
     </row>
   </sheetData>

</xml_diff>